<commit_message>
Add modules and database
</commit_message>
<xml_diff>
--- a/Dev_Plan.xlsx
+++ b/Dev_Plan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B4CDC9-3830-470F-9CB0-DB8C3BC39680}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAA441B-4F30-4E44-9248-884A3D54D950}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,16 +173,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -477,18 +477,18 @@
   <dimension ref="B2:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="8"/>
-    <col min="2" max="2" width="10.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="10.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="18" width="9.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.88671875" style="8"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="10.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="10.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="18" width="9.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -551,40 +551,40 @@
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="6" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
       <c r="J4" s="9" t="s">
         <v>2</v>
       </c>
@@ -596,132 +596,132 @@
       <c r="N4" s="11"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>